<commit_message>
ASU Home Page Tests
</commit_message>
<xml_diff>
--- a/src/main/resources/excelData/WorkBook.xlsx
+++ b/src/main/resources/excelData/WorkBook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dbana\Git\JavaTestScripts\src\main\resources\excelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A7799C-25EF-48AE-B80D-01B728FE4583}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7000E60-92FA-4772-9E34-F171DB1B97C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2304" yWindow="516" windowWidth="17280" windowHeight="9072" xr2:uid="{A5E9F54A-143B-4977-9B27-219227A4E350}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
   <si>
     <t>DegreeType</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>Art History (BA)</t>
+  </si>
+  <si>
+    <t>9563337743</t>
   </si>
 </sst>
 </file>
@@ -472,7 +475,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -530,8 +533,8 @@
       <c r="G2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="1">
-        <v>9563337743</v>
+      <c r="H2" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -556,8 +559,8 @@
       <c r="G3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="1">
-        <v>9563337743</v>
+      <c r="H3" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -582,8 +585,8 @@
       <c r="G4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="1">
-        <v>9563337743</v>
+      <c r="H4" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>